<commit_message>
updated code, finished lab
</commit_message>
<xml_diff>
--- a/lab2temp.xlsx
+++ b/lab2temp.xlsx
@@ -28,134 +28,124 @@
     <t>Quick Sort</t>
   </si>
   <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>1.544e-05</t>
-  </si>
-  <si>
-    <t>1.7644e-05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.146e-05
-</t>
-  </si>
-  <si>
-    <t>91</t>
-  </si>
-  <si>
-    <t>0.000190315</t>
-  </si>
-  <si>
-    <t>7.23126e-05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.04389e-05
-</t>
-  </si>
-  <si>
-    <t>157</t>
-  </si>
-  <si>
-    <t>0.000569756</t>
-  </si>
-  <si>
-    <t>0.000144646</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.000122661
-</t>
-  </si>
-  <si>
-    <t>223</t>
-  </si>
-  <si>
-    <t>0.0012015</t>
-  </si>
-  <si>
-    <t>0.000229513</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.000199888
-</t>
-  </si>
-  <si>
-    <t>289</t>
-  </si>
-  <si>
-    <t>0.00193733</t>
-  </si>
-  <si>
-    <t>0.000301755</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.000259334
-</t>
-  </si>
-  <si>
-    <t>355</t>
-  </si>
-  <si>
-    <t>0.00284782</t>
-  </si>
-  <si>
-    <t>0.000370538</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.000337199
-</t>
-  </si>
-  <si>
-    <t>421</t>
-  </si>
-  <si>
-    <t>0.00398842</t>
-  </si>
-  <si>
-    <t>0.000471187</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.000430707
-</t>
-  </si>
-  <si>
-    <t>487</t>
-  </si>
-  <si>
-    <t>0.00532439</t>
-  </si>
-  <si>
-    <t>0.000541592</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.000482107
-</t>
-  </si>
-  <si>
-    <t>553</t>
-  </si>
-  <si>
-    <t>0.00697669</t>
-  </si>
-  <si>
-    <t>0.000607067</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.000638844
-</t>
-  </si>
-  <si>
-    <t>619</t>
-  </si>
-  <si>
-    <t>0.00852344</t>
-  </si>
-  <si>
-    <t>0.00071324</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0012363
-</t>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>2.09074</t>
+  </si>
+  <si>
+    <t>0.01683</t>
+  </si>
+  <si>
+    <t>0.020335</t>
+  </si>
+  <si>
+    <t>20000</t>
+  </si>
+  <si>
+    <t>8.45289</t>
+  </si>
+  <si>
+    <t>0.036186</t>
+  </si>
+  <si>
+    <t>0.036298</t>
+  </si>
+  <si>
+    <t>30000</t>
+  </si>
+  <si>
+    <t>18.9352</t>
+  </si>
+  <si>
+    <t>0.053639</t>
+  </si>
+  <si>
+    <t>0.056458</t>
+  </si>
+  <si>
+    <t>40000</t>
+  </si>
+  <si>
+    <t>33.1753</t>
+  </si>
+  <si>
+    <t>0.077115</t>
+  </si>
+  <si>
+    <t>0.084508</t>
+  </si>
+  <si>
+    <t>50000</t>
+  </si>
+  <si>
+    <t>53.4929</t>
+  </si>
+  <si>
+    <t>0.100999</t>
+  </si>
+  <si>
+    <t>0.116662</t>
+  </si>
+  <si>
+    <t>60000</t>
+  </si>
+  <si>
+    <t>78.4559</t>
+  </si>
+  <si>
+    <t>0.120201</t>
+  </si>
+  <si>
+    <t>0.133587</t>
+  </si>
+  <si>
+    <t>70000</t>
+  </si>
+  <si>
+    <t>106.37</t>
+  </si>
+  <si>
+    <t>0.14508</t>
+  </si>
+  <si>
+    <t>0.179069</t>
+  </si>
+  <si>
+    <t>80000</t>
+  </si>
+  <si>
+    <t>137.933</t>
+  </si>
+  <si>
+    <t>0.169194</t>
+  </si>
+  <si>
+    <t>0.184616</t>
+  </si>
+  <si>
+    <t>90000</t>
+  </si>
+  <si>
+    <t>171.829</t>
+  </si>
+  <si>
+    <t>0.191406</t>
+  </si>
+  <si>
+    <t>0.231214</t>
+  </si>
+  <si>
+    <t>100000</t>
+  </si>
+  <si>
+    <t>217.711</t>
+  </si>
+  <si>
+    <t>0.215667</t>
+  </si>
+  <si>
+    <t>0.241235</t>
   </si>
 </sst>
 </file>

</xml_diff>